<commit_message>
Attendance of 13_08_2023 and 14_08_2023
Attendance of 13_08_2023 and 14_08_2023
</commit_message>
<xml_diff>
--- a/React-B1-Attendance_Management.xlsx
+++ b/React-B1-Attendance_Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\React-JS\JSLearing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BEE328-B761-4619-9846-1EC9A50BAEBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8025ECC8-FC12-491F-ADDD-6A9F4E8A6177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
@@ -1633,7 +1633,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -2221,9 +2221,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3B6599-6209-4249-B0C6-73BAEC4B8C71}">
   <dimension ref="A1:U742"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3057,45 +3057,125 @@
       <c r="A14" s="4">
         <v>45151</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
+      <c r="B14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="M14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="N14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="O14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="P14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="R14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="S14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="T14" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>45152</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
+      <c r="B15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R15" s="10">
+        <v>16</v>
+      </c>
+      <c r="S15" s="11">
+        <v>10</v>
+      </c>
+      <c r="T15" s="12">
+        <v>6</v>
+      </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
@@ -17834,10 +17914,10 @@
   <dataConsolidate/>
   <dataValidations count="3">
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{D476CE6D-C367-4374-BD3C-CF68DE92BAD3}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:B25 D11:H15 J18:P123 H3 D8:H10 J2:P6 D2:H2 D5:H6 D26:H1048576 F22:H22 D23:H25 D18:H21 M9:P10 J124:K1048576 L9 J8:P8 J11:P15 J9:K10 B26:B1048576 B5:B6 B2 B8:B10 B3:B4 D3:G4" xr:uid="{FD213E24-5FFB-4E4A-B5C9-E949D8E50480}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J18:P123 H3 J15:P15 J2:P6 D2:H2 D5:H6 F22:H22 D23:H1048576 D18:H21 M9:P10 J124:K1048576 L9 J8:P8 B15:B1048576 J9:K10 B2:B6 D3:G4 B8:B13 J11:P13 D8:H13 D15:H15" xr:uid="{FD213E24-5FFB-4E4A-B5C9-E949D8E50480}">
       <formula1>"PRESENT, ABSENT"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 H4 Q2:Q6 Q8:Q123 I1:I1048576 L10 C2:C1048576" xr:uid="{45B840A5-FD6B-42D2-8519-5F95CF7645C3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 H4 Q2:Q6 L10 C2:C1048576 I1:I1048576 Q8:Q13 Q15:Q123" xr:uid="{45B840A5-FD6B-42D2-8519-5F95CF7645C3}">
       <formula1>$U$5:$U$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Attendance of Saturday 26-08-2023 and Sunday 27-08-2023
Attendance of Saturday 26-08-2023 and Sunday 27-08-2023 and practice of coding
</commit_message>
<xml_diff>
--- a/React-B1-Attendance_Management.xlsx
+++ b/React-B1-Attendance_Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\React-JS\JSLearing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A704FD6C-84F5-4926-9D30-8CAECCD0DE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB59F8D0-3A91-4C6F-9235-9642DED022FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
@@ -5310,17 +5310,11 @@
       <c r="A27" s="4">
         <v>45164</v>
       </c>
-      <c r="Q27" s="3"/>
-      <c r="R27" s="3"/>
-      <c r="S27" s="3"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>45165</v>
       </c>
-      <c r="Q28" s="3"/>
-      <c r="R28" s="3"/>
-      <c r="S28" s="3"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
@@ -9803,7 +9797,7 @@
   <dataConsolidate/>
   <dataValidations count="2">
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{D476CE6D-C367-4374-BD3C-CF68DE92BAD3}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1:V1048576 N24 B1:P23 B26:P1048576 B24:M25 O24:P25 N25" xr:uid="{45B840A5-FD6B-42D2-8519-5F95CF7645C3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1:V1048576 B1:P26 B29:P1048576" xr:uid="{45B840A5-FD6B-42D2-8519-5F95CF7645C3}">
       <formula1>$T$5:$T$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Attendance of 17/18/19 SEPT 2023
Attendance of 17/18/19 SEPT 2023
</commit_message>
<xml_diff>
--- a/React-B1-Attendance_Management.xlsx
+++ b/React-B1-Attendance_Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\React-JS\JSLearing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8D2866-D7AA-4BC8-8BDA-CDEEC15AB0DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F6B673-7B76-430D-B942-EA62CFDFC250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
@@ -5996,7 +5996,55 @@
         </r>
       </text>
     </comment>
-    <comment ref="D48" authorId="0" shapeId="0" xr:uid="{8C0948D1-6569-448E-877D-6C1BAED0CD6A}">
+    <comment ref="E48" authorId="0" shapeId="0" xr:uid="{6CE3520A-3696-4274-A8B5-4D0F927AA31E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not Responded</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H48" authorId="0" shapeId="0" xr:uid="{3D99DE63-8DD3-474E-979C-C6F7BD4E598F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Extra Studies</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I48" authorId="0" shapeId="0" xr:uid="{EA01C709-939D-486F-864E-108BDD7F5CAC}">
       <text>
         <r>
           <rPr>
@@ -6020,7 +6068,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="E48" authorId="0" shapeId="0" xr:uid="{6CE3520A-3696-4274-A8B5-4D0F927AA31E}">
+    <comment ref="J48" authorId="0" shapeId="0" xr:uid="{0145C9C1-D06A-4740-805A-B80546FD015C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Extra Studies</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K48" authorId="0" shapeId="0" xr:uid="{410AB793-6742-430F-8852-0BA56C550D95}">
       <text>
         <r>
           <rPr>
@@ -6044,7 +6116,103 @@
         </r>
       </text>
     </comment>
-    <comment ref="H48" authorId="0" shapeId="0" xr:uid="{3D99DE63-8DD3-474E-979C-C6F7BD4E598F}">
+    <comment ref="L48" authorId="0" shapeId="0" xr:uid="{9AC9E368-CC8A-4FF1-8579-5ED9C4FDAAAC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Network issue occurred joined the metting only foe 10 min</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O48" authorId="0" shapeId="0" xr:uid="{E768848A-46CE-4892-9C95-92FDDCCA80D5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not Responded</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C50" authorId="0" shapeId="0" xr:uid="{757930A9-1E82-455F-8360-4509CCCD26F0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not Responded</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E50" authorId="0" shapeId="0" xr:uid="{C468986F-5C1E-4E72-9339-2FA8973133D1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not Responded</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H50" authorId="0" shapeId="0" xr:uid="{D73C652B-4F50-4A25-B694-8963AF164568}">
       <text>
         <r>
           <rPr>
@@ -6068,31 +6236,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="I48" authorId="0" shapeId="0" xr:uid="{EA01C709-939D-486F-864E-108BDD7F5CAC}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Parth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Joined Only 1st session</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J48" authorId="0" shapeId="0" xr:uid="{0145C9C1-D06A-4740-805A-B80546FD015C}">
+    <comment ref="I50" authorId="0" shapeId="0" xr:uid="{909DBE35-205D-4FCC-96D2-3BD3AC91A463}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Not Responded</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J50" authorId="0" shapeId="0" xr:uid="{320C7517-DA85-44C5-8357-445445F11FBB}">
       <text>
         <r>
           <rPr>
@@ -6116,7 +6284,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K48" authorId="0" shapeId="0" xr:uid="{410AB793-6742-430F-8852-0BA56C550D95}">
+    <comment ref="K50" authorId="0" shapeId="0" xr:uid="{45259C79-D789-4A81-AD01-34BFB2CFFAD7}">
       <text>
         <r>
           <rPr>
@@ -6140,7 +6308,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L48" authorId="0" shapeId="0" xr:uid="{9AC9E368-CC8A-4FF1-8579-5ED9C4FDAAAC}">
+    <comment ref="L50" authorId="0" shapeId="0" xr:uid="{21E583A2-C8DA-476E-866C-ECB36AF7F0F5}">
       <text>
         <r>
           <rPr>
@@ -6161,6 +6329,78 @@
           </rPr>
           <t xml:space="preserve">
 Network issue occurred joined the metting only foe 10 min</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N50" authorId="0" shapeId="0" xr:uid="{CC8B6101-3785-49ED-8C7D-D31F9A3D155E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not Responded</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O50" authorId="0" shapeId="0" xr:uid="{5701182F-AC76-4DBE-A59E-CBB02E7006DB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not Responded</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P50" authorId="0" shapeId="0" xr:uid="{1D7814A8-81F9-4FC7-B4C3-CD80401AD5A3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Parth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not Responded</t>
         </r>
       </text>
     </comment>
@@ -6169,7 +6409,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -6253,6 +6493,9 @@
   </si>
   <si>
     <t>Common-Off</t>
+  </si>
+  <si>
+    <t>Ganesh Chaturthi Holiday</t>
   </si>
 </sst>
 </file>
@@ -6795,8 +7038,8 @@
   <dimension ref="A1:V742"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -9667,7 +9910,7 @@
       <c r="C48" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D48" s="14" t="s">
+      <c r="D48" s="11" t="s">
         <v>2</v>
       </c>
       <c r="E48" s="13" t="s">
@@ -9700,7 +9943,7 @@
       <c r="N48" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="O48" s="11" t="s">
+      <c r="O48" s="13" t="s">
         <v>1</v>
       </c>
       <c r="P48" s="11" t="s">
@@ -9720,25 +9963,178 @@
       <c r="A49" s="12">
         <v>45186</v>
       </c>
-      <c r="Q49" s="11"/>
-      <c r="R49" s="11"/>
-      <c r="S49" s="11"/>
+      <c r="B49" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F49" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G49" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H49" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I49" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J49" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="K49" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="L49" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="M49" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="N49" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="O49" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="P49" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q49" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="R49" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="S49" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" s="12">
         <v>45187</v>
       </c>
-      <c r="Q50" s="11"/>
-      <c r="R50" s="11"/>
-      <c r="S50" s="11"/>
+      <c r="B50" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E50" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F50" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G50" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H50" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I50" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="J50" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="K50" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="L50" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="M50" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="N50" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="O50" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="P50" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q50" s="1">
+        <v>15</v>
+      </c>
+      <c r="R50" s="2">
+        <v>5</v>
+      </c>
+      <c r="S50" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" s="12">
         <v>45188</v>
       </c>
-      <c r="Q51" s="11"/>
-      <c r="R51" s="11"/>
-      <c r="S51" s="11"/>
+      <c r="B51" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E51" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F51" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G51" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H51" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I51" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="J51" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="K51" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="L51" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="M51" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="N51" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="O51" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="P51" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q51" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="R51" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="S51" s="15" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52" s="12">
@@ -14053,7 +14449,7 @@
   <dataConsolidate/>
   <dataValidations count="2">
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{D476CE6D-C367-4374-BD3C-CF68DE92BAD3}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1:V1048576 B1:P30 B32:P40 C42:S42 B42:B1048576 C43:P1048576" xr:uid="{45B840A5-FD6B-42D2-8519-5F95CF7645C3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1:V1048576 B1:P30 B32:P40 C42:S42 C49:S49 C43:P48 B42:B1048576 C50:P50 C52:P1048576 C51:S51" xr:uid="{45B840A5-FD6B-42D2-8519-5F95CF7645C3}">
       <formula1>$T$5:$T$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>